<commit_message>
Import manual TUS and export new sheet
</commit_message>
<xml_diff>
--- a/Output/instrument_data_all_years/tus.xlsx
+++ b/Output/instrument_data_all_years/tus.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="195">
   <si>
     <t>country</t>
   </si>
   <si>
-    <t>iso3c</t>
+    <t>country_code</t>
   </si>
   <si>
     <t>year</t>
@@ -113,34 +113,160 @@
     <t>26</t>
   </si>
   <si>
-    <t>Afghanistan</t>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
   <si>
     <t>Argentina</t>
   </si>
   <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
     <t>Belgium</t>
   </si>
   <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
     <t>Canada</t>
   </si>
   <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
     <t>Colombia</t>
   </si>
   <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
     <t>Ethiopia</t>
   </si>
   <si>
+    <t>Georgia</t>
+  </si>
+  <si>
     <t>Germany</t>
   </si>
   <si>
     <t>Greece</t>
   </si>
   <si>
-    <t>Iran</t>
-  </si>
-  <si>
-    <t>Kyrgyz Republic</t>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Iran, Islamic Rep.</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Korea, Rep.</t>
   </si>
   <si>
     <t>Kyrgyzstan</t>
@@ -149,19 +275,37 @@
     <t>Luxembourg</t>
   </si>
   <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
     <t>Mexico</t>
   </si>
   <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>Palestine</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
     <t>Poland</t>
   </si>
   <si>
+    <t>Portugal</t>
+  </si>
+  <si>
     <t>Qatar</t>
   </si>
   <si>
-    <t>Republic of Korea</t>
-  </si>
-  <si>
-    <t>State of Palestine</t>
+    <t>Serbia</t>
   </si>
   <si>
     <t>Switzerland</t>
@@ -176,7 +320,13 @@
     <t>Turkey</t>
   </si>
   <si>
-    <t>United Republic of Tanzania</t>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States</t>
   </si>
   <si>
     <t>United States of America</t>
@@ -185,52 +335,115 @@
     <t>Uruguay</t>
   </si>
   <si>
-    <t>AFG</t>
+    <t>Vietnam</t>
   </si>
   <si>
     <t>ARG</t>
   </si>
   <si>
+    <t>BGD</t>
+  </si>
+  <si>
+    <t>BLR</t>
+  </si>
+  <si>
     <t>BEL</t>
   </si>
   <si>
+    <t>BLZ</t>
+  </si>
+  <si>
+    <t>BRA</t>
+  </si>
+  <si>
+    <t>CMR</t>
+  </si>
+  <si>
     <t>CAN</t>
   </si>
   <si>
+    <t>CHL</t>
+  </si>
+  <si>
+    <t>CHN</t>
+  </si>
+  <si>
     <t>COL</t>
   </si>
   <si>
+    <t>CRI</t>
+  </si>
+  <si>
+    <t>DOM</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
     <t>ETH</t>
   </si>
   <si>
+    <t>GEO</t>
+  </si>
+  <si>
     <t>DEU</t>
   </si>
   <si>
     <t>GRC</t>
   </si>
   <si>
+    <t>IND</t>
+  </si>
+  <si>
     <t>IRN</t>
   </si>
   <si>
+    <t>ITA</t>
+  </si>
+  <si>
+    <t>JPN</t>
+  </si>
+  <si>
+    <t>KOR</t>
+  </si>
+  <si>
     <t>KGZ</t>
   </si>
   <si>
     <t>LUX</t>
   </si>
   <si>
+    <t>MUS</t>
+  </si>
+  <si>
     <t>MEX</t>
   </si>
   <si>
+    <t>MNG</t>
+  </si>
+  <si>
+    <t>NLD</t>
+  </si>
+  <si>
+    <t>MKD</t>
+  </si>
+  <si>
+    <t>PSE</t>
+  </si>
+  <si>
+    <t>PRY</t>
+  </si>
+  <si>
     <t>POL</t>
   </si>
   <si>
+    <t>PRT</t>
+  </si>
+  <si>
     <t>QAT</t>
   </si>
   <si>
-    <t>KOR</t>
-  </si>
-  <si>
-    <t>PSE</t>
+    <t>SRB</t>
   </si>
   <si>
     <t>CHE</t>
@@ -245,21 +458,39 @@
     <t>TUR</t>
   </si>
   <si>
+    <t>UGA</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
     <t>USA</t>
   </si>
   <si>
     <t>URY</t>
   </si>
   <si>
-    <t>2020</t>
+    <t>VNM</t>
   </si>
   <si>
     <t>2013</t>
   </si>
   <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2014-15</t>
+  </si>
+  <si>
     <t>2013-14</t>
   </si>
   <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
     <t>2014</t>
   </si>
   <si>
@@ -269,31 +500,103 @@
     <t>2012-13</t>
   </si>
   <si>
-    <t>2014-15</t>
-  </si>
-  <si>
-    <t>2015</t>
-  </si>
-  <si>
-    <t>TUS 2020 (https://www2.unwomen.org/-/media/field%20office%20eseasia/docs/publications/2020/05/timeusesurveymay2020.pdf?la=en&amp;vs=3719)</t>
-  </si>
-  <si>
-    <t>Time Use Survey 2010, 2015</t>
-  </si>
-  <si>
-    <t>Integrated Labour Force Survey - Time Use Survey Module 2014</t>
+    <t>2016-17</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2019-2021</t>
+  </si>
+  <si>
+    <t>2020-21</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2018-19</t>
+  </si>
+  <si>
+    <t>2017-18</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2022</t>
   </si>
   <si>
     <t>Time Use Survey</t>
   </si>
   <si>
+    <t>Module of household survey</t>
+  </si>
+  <si>
+    <t>Encuesta Nacional sobre Uso del Tiempo</t>
+  </si>
+  <si>
+    <t>Encuesta Nacional de Uso del Tiempo 2012-2013</t>
+  </si>
+  <si>
+    <t>Module of living conditions survey</t>
+  </si>
+  <si>
+    <t>Encuesta Sobre Uso del Tiempo</t>
+  </si>
+  <si>
+    <t>Not specified</t>
+  </si>
+  <si>
+    <t>Module of household budget survey</t>
+  </si>
+  <si>
+    <t>Time Use Survey 2022</t>
+  </si>
+  <si>
+    <t>https://unstats.un.org/unsd/demographic-social/time-use/</t>
+  </si>
+  <si>
+    <t>https://data.unwomen.org/publications/bangladesh-time-use-survey-2021</t>
+  </si>
+  <si>
+    <t>https://data.unwomen.org/sites/default/files/documents/Publications/Measuring%20time%20use.pdf</t>
+  </si>
+  <si>
+    <t>https://catalog.ihsn.org/catalog/7768</t>
+  </si>
+  <si>
+    <t>https://catalog.ihsn.org/catalog/7172</t>
+  </si>
+  <si>
+    <t>https://www.stat.ee/en/find-statistics/statistics-theme/well-being/time-use</t>
+  </si>
+  <si>
+    <t>https://data.unwomen.org/publications/time-use-survey-georgia-2020-2021</t>
+  </si>
+  <si>
     <t>https://unstats.un.org/unsd/gender/timeuse and manual ODW check of NSO websites</t>
   </si>
   <si>
-    <t>https://unstats.un.org/unsd/demographic-social/time-use/</t>
+    <t>https://catalog.ihsn.org/catalog/8344</t>
+  </si>
+  <si>
+    <t>https://digitaal.scp.nl/timeuse1/background-of-the-time-use-survey/</t>
+  </si>
+  <si>
+    <t>https://catalog.ihsn.org/catalog/7783</t>
+  </si>
+  <si>
+    <t>https://www.stat.gov.rs/en-us/oblasti/stanovnistvo/statistika-polova/</t>
+  </si>
+  <si>
+    <t>https://catalog.ihsn.org/catalog/11322</t>
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>See p. 142</t>
   </si>
 </sst>
 </file>
@@ -373,25 +676,25 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="F2" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
       <c r="H2" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3">
@@ -399,25 +702,25 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E3" t="e">
-        <v>#N/A</v>
+        <v>154</v>
+      </c>
+      <c r="E3" t="s">
+        <v>171</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>181</v>
       </c>
       <c r="H3" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4">
@@ -425,25 +728,25 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="e">
-        <v>#N/A</v>
+        <v>155</v>
+      </c>
+      <c r="E4" t="s">
+        <v>171</v>
       </c>
       <c r="F4" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5">
@@ -451,25 +754,25 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" t="e">
-        <v>#N/A</v>
+        <v>156</v>
+      </c>
+      <c r="E5" t="s">
+        <v>171</v>
       </c>
       <c r="F5" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G5" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6">
@@ -477,25 +780,25 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" t="e">
-        <v>#N/A</v>
+        <v>157</v>
+      </c>
+      <c r="E6" t="s">
+        <v>172</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G6" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7">
@@ -503,25 +806,25 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="e">
-        <v>#N/A</v>
+        <v>158</v>
+      </c>
+      <c r="E7" t="s">
+        <v>172</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8">
@@ -529,25 +832,25 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" t="e">
-        <v>#N/A</v>
+        <v>159</v>
+      </c>
+      <c r="E8" t="s">
+        <v>172</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G8" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="9">
@@ -555,25 +858,25 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" t="e">
-        <v>#N/A</v>
+        <v>159</v>
+      </c>
+      <c r="E9" t="s">
+        <v>171</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G9" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="H9" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10">
@@ -581,25 +884,25 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" t="e">
-        <v>#N/A</v>
+        <v>160</v>
+      </c>
+      <c r="E10" t="s">
+        <v>171</v>
       </c>
       <c r="F10" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G10" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="H10" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11">
@@ -607,25 +910,25 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" t="e">
-        <v>#N/A</v>
+        <v>157</v>
+      </c>
+      <c r="E11" t="s">
+        <v>173</v>
       </c>
       <c r="F11" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G11" t="s">
-        <v>92</v>
+        <v>183</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12">
@@ -633,25 +936,25 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>182</v>
       </c>
       <c r="H12" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13">
@@ -659,25 +962,25 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13" t="e">
-        <v>#N/A</v>
+        <v>161</v>
+      </c>
+      <c r="E13" t="s">
+        <v>174</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G13" t="s">
-        <v>92</v>
+        <v>184</v>
       </c>
       <c r="H13" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14">
@@ -685,25 +988,25 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" t="e">
-        <v>#N/A</v>
+        <v>162</v>
+      </c>
+      <c r="E14" t="s">
+        <v>171</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G14" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H14" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15">
@@ -711,25 +1014,25 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" t="e">
-        <v>#N/A</v>
+        <v>158</v>
+      </c>
+      <c r="E15" t="s">
+        <v>172</v>
       </c>
       <c r="F15" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G15" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H15" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16">
@@ -737,25 +1040,25 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="e">
-        <v>#N/A</v>
+        <v>163</v>
+      </c>
+      <c r="E16" t="s">
+        <v>172</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G16" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H16" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17">
@@ -763,25 +1066,25 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>121</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
-      </c>
-      <c r="E17" t="e">
-        <v>#N/A</v>
+        <v>164</v>
+      </c>
+      <c r="E17" t="s">
+        <v>171</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G17" t="s">
-        <v>92</v>
+        <v>185</v>
       </c>
       <c r="H17" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="18">
@@ -789,25 +1092,25 @@
         <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" t="e">
-        <v>#N/A</v>
+        <v>153</v>
+      </c>
+      <c r="E18" t="s">
+        <v>171</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G18" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="H18" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19">
@@ -815,25 +1118,25 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" t="e">
-        <v>#N/A</v>
+        <v>165</v>
+      </c>
+      <c r="E19" t="s">
+        <v>171</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G19" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20">
@@ -841,25 +1144,25 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" t="e">
-        <v>#N/A</v>
+        <v>161</v>
+      </c>
+      <c r="E20" t="s">
+        <v>171</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G20" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H20" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21">
@@ -867,25 +1170,25 @@
         <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>156</v>
       </c>
       <c r="E21" t="s">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G21" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
       <c r="H21" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22">
@@ -893,25 +1196,25 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>126</v>
       </c>
       <c r="D22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E22" t="e">
-        <v>#N/A</v>
+        <v>166</v>
+      </c>
+      <c r="E22" t="s">
+        <v>171</v>
       </c>
       <c r="F22" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H22" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23">
@@ -919,25 +1222,25 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>127</v>
       </c>
       <c r="D23" t="s">
-        <v>85</v>
-      </c>
-      <c r="E23" t="e">
-        <v>#N/A</v>
+        <v>155</v>
+      </c>
+      <c r="E23" t="s">
+        <v>171</v>
       </c>
       <c r="F23" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G23" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="H23" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24">
@@ -945,25 +1248,25 @@
         <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" t="e">
-        <v>#N/A</v>
+        <v>156</v>
+      </c>
+      <c r="E24" t="s">
+        <v>171</v>
       </c>
       <c r="F24" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G24" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H24" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25">
@@ -971,25 +1274,25 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
       <c r="D25" t="s">
-        <v>80</v>
-      </c>
-      <c r="E25" t="e">
-        <v>#N/A</v>
+        <v>163</v>
+      </c>
+      <c r="E25" t="s">
+        <v>171</v>
       </c>
       <c r="F25" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G25" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="H25" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26">
@@ -997,25 +1300,25 @@
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
-      </c>
-      <c r="E26" t="e">
-        <v>#N/A</v>
+        <v>159</v>
+      </c>
+      <c r="E26" t="s">
+        <v>171</v>
       </c>
       <c r="F26" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G26" t="s">
-        <v>92</v>
+        <v>180</v>
       </c>
       <c r="H26" t="s">
-        <v>93</v>
+        <v>193</v>
       </c>
     </row>
     <row r="27">
@@ -1023,25 +1326,779 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E27" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" t="s">
+        <v>171</v>
+      </c>
+      <c r="G27" t="s">
+        <v>187</v>
+      </c>
+      <c r="H27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E28" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G28" t="s">
+        <v>180</v>
+      </c>
+      <c r="H28" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" t="s">
+        <v>167</v>
+      </c>
+      <c r="E29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" t="s">
+        <v>171</v>
+      </c>
+      <c r="G29" t="s">
+        <v>182</v>
+      </c>
+      <c r="H29" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F30" t="s">
+        <v>171</v>
+      </c>
+      <c r="G30" t="s">
+        <v>180</v>
+      </c>
+      <c r="H30" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" t="s">
+        <v>171</v>
+      </c>
+      <c r="F31" t="s">
+        <v>171</v>
+      </c>
+      <c r="G31" t="s">
+        <v>188</v>
+      </c>
+      <c r="H31" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" t="s">
+        <v>166</v>
+      </c>
+      <c r="E32" t="s">
+        <v>171</v>
+      </c>
+      <c r="F32" t="s">
+        <v>171</v>
+      </c>
+      <c r="G32" t="s">
+        <v>182</v>
+      </c>
+      <c r="H32" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" t="s">
+        <v>171</v>
+      </c>
+      <c r="F33" t="s">
+        <v>171</v>
+      </c>
+      <c r="G33" t="s">
+        <v>189</v>
+      </c>
+      <c r="H33" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" t="s">
+        <v>171</v>
+      </c>
+      <c r="F34" t="s">
+        <v>171</v>
+      </c>
+      <c r="G34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H34" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" t="s">
+        <v>161</v>
+      </c>
+      <c r="E35" t="s">
+        <v>171</v>
+      </c>
+      <c r="F35" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D36" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36" t="s">
+        <v>176</v>
+      </c>
+      <c r="F36" t="s">
+        <v>171</v>
+      </c>
+      <c r="G36" t="s">
+        <v>190</v>
+      </c>
+      <c r="H36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" t="s">
+        <v>153</v>
+      </c>
+      <c r="E37" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" t="s">
+        <v>171</v>
+      </c>
+      <c r="G37" t="s">
+        <v>180</v>
+      </c>
+      <c r="H37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" t="s">
+        <v>171</v>
+      </c>
+      <c r="F38" t="s">
+        <v>171</v>
+      </c>
+      <c r="G38" t="s">
+        <v>182</v>
+      </c>
+      <c r="H38" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>96</v>
+      </c>
+      <c r="C39" t="s">
+        <v>142</v>
+      </c>
+      <c r="D39" t="s">
+        <v>161</v>
+      </c>
+      <c r="E39" t="s">
+        <v>177</v>
+      </c>
+      <c r="F39" t="s">
+        <v>171</v>
+      </c>
+      <c r="G39" t="s">
+        <v>182</v>
+      </c>
+      <c r="H39" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" t="s">
+        <v>97</v>
+      </c>
+      <c r="C40" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" t="s">
+        <v>154</v>
+      </c>
+      <c r="E40" t="s">
+        <v>171</v>
+      </c>
+      <c r="F40" t="s">
+        <v>171</v>
+      </c>
+      <c r="G40" t="s">
+        <v>191</v>
+      </c>
+      <c r="H40" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" t="s">
+        <v>153</v>
+      </c>
+      <c r="E41" t="s">
+        <v>171</v>
+      </c>
+      <c r="F41" t="s">
+        <v>171</v>
+      </c>
+      <c r="G41" t="s">
+        <v>180</v>
+      </c>
+      <c r="H41" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" t="s">
+        <v>145</v>
+      </c>
+      <c r="D42" t="s">
+        <v>159</v>
+      </c>
+      <c r="E42" t="s">
+        <v>171</v>
+      </c>
+      <c r="F42" t="s">
+        <v>171</v>
+      </c>
+      <c r="G42" t="s">
+        <v>187</v>
+      </c>
+      <c r="H42" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" t="s">
+        <v>145</v>
+      </c>
+      <c r="D43" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" t="s">
+        <v>178</v>
+      </c>
+      <c r="F43" t="s">
+        <v>171</v>
+      </c>
+      <c r="G43" t="s">
+        <v>182</v>
+      </c>
+      <c r="H43" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C44" t="s">
+        <v>146</v>
+      </c>
+      <c r="D44" t="s">
+        <v>159</v>
+      </c>
+      <c r="E44" t="s">
+        <v>171</v>
+      </c>
+      <c r="F44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G44" t="s">
+        <v>180</v>
+      </c>
+      <c r="H44" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" t="s">
+        <v>171</v>
+      </c>
+      <c r="F45" t="s">
+        <v>171</v>
+      </c>
+      <c r="G45" t="s">
+        <v>180</v>
+      </c>
+      <c r="H45" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" t="s">
+        <v>168</v>
+      </c>
+      <c r="E46" t="s">
+        <v>171</v>
+      </c>
+      <c r="F46" t="s">
+        <v>171</v>
+      </c>
+      <c r="G46" t="s">
+        <v>182</v>
+      </c>
+      <c r="H46" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" t="s">
+        <v>157</v>
+      </c>
+      <c r="E47" t="s">
+        <v>171</v>
+      </c>
+      <c r="F47" t="s">
+        <v>171</v>
+      </c>
+      <c r="G47" t="s">
+        <v>182</v>
+      </c>
+      <c r="H47" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" t="s">
+        <v>150</v>
+      </c>
+      <c r="D48" t="s">
+        <v>153</v>
+      </c>
+      <c r="E48" t="s">
+        <v>171</v>
+      </c>
+      <c r="F48" t="s">
+        <v>171</v>
+      </c>
+      <c r="G48" t="s">
+        <v>180</v>
+      </c>
+      <c r="H48" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" t="s">
+        <v>150</v>
+      </c>
+      <c r="D49" t="s">
+        <v>159</v>
+      </c>
+      <c r="E49" t="s">
+        <v>171</v>
+      </c>
+      <c r="F49" t="s">
+        <v>171</v>
+      </c>
+      <c r="G49" t="s">
+        <v>180</v>
+      </c>
+      <c r="H49" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" t="s">
+        <v>105</v>
+      </c>
+      <c r="C50" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" t="s">
+        <v>157</v>
+      </c>
+      <c r="E50" t="s">
+        <v>171</v>
+      </c>
+      <c r="F50" t="s">
+        <v>171</v>
+      </c>
+      <c r="G50" t="s">
+        <v>182</v>
+      </c>
+      <c r="H50" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
         <v>56</v>
       </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>80</v>
-      </c>
-      <c r="E27" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="F27" t="s">
-        <v>90</v>
-      </c>
-      <c r="G27" t="s">
-        <v>92</v>
-      </c>
-      <c r="H27" t="s">
-        <v>93</v>
+      <c r="B51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" t="s">
+        <v>163</v>
+      </c>
+      <c r="E51" t="s">
+        <v>171</v>
+      </c>
+      <c r="F51" t="s">
+        <v>171</v>
+      </c>
+      <c r="G51" t="s">
+        <v>182</v>
+      </c>
+      <c r="H51" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" t="s">
+        <v>150</v>
+      </c>
+      <c r="D52" t="s">
+        <v>158</v>
+      </c>
+      <c r="E52" t="s">
+        <v>171</v>
+      </c>
+      <c r="F52" t="s">
+        <v>171</v>
+      </c>
+      <c r="G52" t="s">
+        <v>182</v>
+      </c>
+      <c r="H52" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" t="s">
+        <v>169</v>
+      </c>
+      <c r="E53" t="s">
+        <v>171</v>
+      </c>
+      <c r="F53" t="s">
+        <v>171</v>
+      </c>
+      <c r="G53" t="s">
+        <v>182</v>
+      </c>
+      <c r="H53" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" t="s">
+        <v>166</v>
+      </c>
+      <c r="E54" t="s">
+        <v>171</v>
+      </c>
+      <c r="F54" t="s">
+        <v>171</v>
+      </c>
+      <c r="G54" t="s">
+        <v>182</v>
+      </c>
+      <c r="H54" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>60</v>
+      </c>
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" t="s">
+        <v>151</v>
+      </c>
+      <c r="D55" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55" t="s">
+        <v>171</v>
+      </c>
+      <c r="F55" t="s">
+        <v>171</v>
+      </c>
+      <c r="G55" t="s">
+        <v>180</v>
+      </c>
+      <c r="H55" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" t="s">
+        <v>152</v>
+      </c>
+      <c r="D56" t="s">
+        <v>170</v>
+      </c>
+      <c r="E56" t="s">
+        <v>179</v>
+      </c>
+      <c r="F56" t="s">
+        <v>171</v>
+      </c>
+      <c r="G56" t="s">
+        <v>192</v>
+      </c>
+      <c r="H56" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>